<commit_message>
myrs and assessments v2 (#230)
* initial commit

* assessments

* forecast report

* small fix
</commit_message>
<xml_diff>
--- a/next/app/model-year-report/lib/templates/assessment_template.xlsx
+++ b/next/app/model-year-report/lib/templates/assessment_template.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE639786-D161-DA41-AE12-A576554CDB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E110C283-C2D6-E949-89B1-7B5AB57CABCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="2400" windowWidth="27640" windowHeight="16940" xr2:uid="{596842B5-1F9C-BB4A-9EA7-2707F0F20405}"/>
+    <workbookView xWindow="1440" yWindow="2100" windowWidth="32280" windowHeight="16940" xr2:uid="{596842B5-1F9C-BB4A-9EA7-2707F0F20405}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
-    <sheet name="Compliance Reductions" sheetId="2" r:id="rId2"/>
-    <sheet name="Section 19(1)(a)" sheetId="4" r:id="rId3"/>
-    <sheet name="Section 19(1)(b)" sheetId="3" r:id="rId4"/>
-    <sheet name="Section 19(1)(c) - Part 1" sheetId="5" r:id="rId5"/>
-    <sheet name="Section 19(1)(c) - Part 2" sheetId="6" r:id="rId6"/>
-    <sheet name="Section 19(1)(e) - Previous" sheetId="7" r:id="rId7"/>
-    <sheet name="Section 19(1)(e) - Current" sheetId="9" r:id="rId8"/>
-    <sheet name="Section 19(1)(f)" sheetId="8" r:id="rId9"/>
+    <sheet name="Compliance Ratio Reductions" sheetId="2" r:id="rId2"/>
+    <sheet name="Beginning Balance" sheetId="10" r:id="rId3"/>
+    <sheet name="Credits" sheetId="6" r:id="rId4"/>
+    <sheet name="Previous Adjustments" sheetId="7" r:id="rId5"/>
+    <sheet name="Current Adjustments" sheetId="9" r:id="rId6"/>
+    <sheet name="Offsets and Transfers Away" sheetId="5" r:id="rId7"/>
+    <sheet name="Final Ending Balance" sheetId="3" r:id="rId8"/>
+    <sheet name="Statement(s)" sheetId="4" r:id="rId9"/>
+    <sheet name="Divisor" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
   <si>
     <t>Supplier Name</t>
   </si>
@@ -52,9 +53,6 @@
     <t>Model Year</t>
   </si>
   <si>
-    <t>The ZEV class of credits that should be used first when offsetting debits of the unspecified ZEV class</t>
-  </si>
-  <si>
     <t>Compliance Ratio</t>
   </si>
   <si>
@@ -79,13 +77,19 @@
     <t>Offset or Transfer Away</t>
   </si>
   <si>
-    <t>Reference Id</t>
-  </si>
-  <si>
-    <t>Legacy Reference Id</t>
-  </si>
-  <si>
     <t>Credit Type</t>
+  </si>
+  <si>
+    <t>ZEV Class Ordering</t>
+  </si>
+  <si>
+    <t>Divisor</t>
+  </si>
+  <si>
+    <t>Final Number of Units</t>
+  </si>
+  <si>
+    <t>Initial Number of Units</t>
   </si>
 </sst>
 </file>
@@ -474,7 +478,8 @@
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
-    <col min="4" max="4" width="86.83203125" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -485,13 +490,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91F418E-62AA-B84B-ABCE-E4D97A035535}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -513,7 +530,47 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70438796-C504-964A-BE49-E27234E80981}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -522,13 +579,10 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -536,50 +590,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A603B588-451E-DE47-B4C5-80CCA31AA744}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="135.5" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59281AEA-3AA5-0C4E-A67E-4D6171492622}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092B32A8-1A64-2347-99F3-32905DDC8385}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -588,95 +627,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240610B3-BA6F-EA4D-8E64-BC14F2315C65}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092B32A8-1A64-2347-99F3-32905DDC8385}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63D4D29-49CB-FE47-AAC8-5E814C359DDB}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -693,19 +643,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -713,7 +663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F2F3A0-C836-3C4C-9B76-FCF87CCE7131}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -730,19 +680,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -750,15 +700,95 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240610B3-BA6F-EA4D-8E64-BC14F2315C65}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59281AEA-3AA5-0C4E-A67E-4D6171492622}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EE9819-10C8-664D-85A7-E78A635E958F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A603B588-451E-DE47-B4C5-80CCA31AA744}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="166" customWidth="1"/>
+    <col min="1" max="1" width="135.5" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
242: myr changes (#277)
</commit_message>
<xml_diff>
--- a/next/app/model-year-report/lib/templates/assessment_template.xlsx
+++ b/next/app/model-year-report/lib/templates/assessment_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/zeva/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E110C283-C2D6-E949-89B1-7B5AB57CABCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B1F051-C09F-0640-B40A-7D67FD51B4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="2100" windowWidth="32280" windowHeight="16940" xr2:uid="{596842B5-1F9C-BB4A-9EA7-2707F0F20405}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
   <si>
     <t>Supplier Name</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Initial Number of Units</t>
+  </si>
+  <si>
+    <t>Compliant</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F98C4F-709F-BE41-A61C-7C5BE18E78C9}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,9 +483,10 @@
     <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,6 +498,9 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge release/0.4.0 to main (#294)
</commit_message>
<xml_diff>
--- a/next/app/model-year-report/lib/templates/assessment_template.xlsx
+++ b/next/app/model-year-report/lib/templates/assessment_template.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/zeva/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FD9171-12EA-384D-B7EE-67E28DCF404E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B1F051-C09F-0640-B40A-7D67FD51B4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8600" yWindow="2400" windowWidth="27640" windowHeight="16940" xr2:uid="{596842B5-1F9C-BB4A-9EA7-2707F0F20405}"/>
+    <workbookView xWindow="1440" yWindow="2100" windowWidth="32280" windowHeight="16940" xr2:uid="{596842B5-1F9C-BB4A-9EA7-2707F0F20405}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
-    <sheet name="Compliance Reductions" sheetId="2" r:id="rId2"/>
-    <sheet name="Section 19(1)(a)" sheetId="4" r:id="rId3"/>
-    <sheet name="Section 19(1)(b)" sheetId="3" r:id="rId4"/>
-    <sheet name="Section 19(1)(c) - Part 1" sheetId="5" r:id="rId5"/>
-    <sheet name="Section 19(1)(c) - Part 2" sheetId="6" r:id="rId6"/>
-    <sheet name="Section 19(1)(e)" sheetId="7" r:id="rId7"/>
-    <sheet name="Section 19(1)(f)" sheetId="8" r:id="rId8"/>
+    <sheet name="Compliance Ratio Reductions" sheetId="2" r:id="rId2"/>
+    <sheet name="Beginning Balance" sheetId="10" r:id="rId3"/>
+    <sheet name="Credits" sheetId="6" r:id="rId4"/>
+    <sheet name="Previous Adjustments" sheetId="7" r:id="rId5"/>
+    <sheet name="Current Adjustments" sheetId="9" r:id="rId6"/>
+    <sheet name="Offsets and Transfers Away" sheetId="5" r:id="rId7"/>
+    <sheet name="Final Ending Balance" sheetId="3" r:id="rId8"/>
+    <sheet name="Statement(s)" sheetId="4" r:id="rId9"/>
+    <sheet name="Divisor" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
   <si>
     <t>Supplier Name</t>
   </si>
@@ -51,9 +53,6 @@
     <t>Model Year</t>
   </si>
   <si>
-    <t>The ZEV class of credits that should be used first when offsetting debits of the unspecified ZEV class</t>
-  </si>
-  <si>
     <t>Compliance Ratio</t>
   </si>
   <si>
@@ -78,13 +77,22 @@
     <t>Offset or Transfer Away</t>
   </si>
   <si>
-    <t>Reference Id</t>
-  </si>
-  <si>
-    <t>Legacy Reference Id</t>
-  </si>
-  <si>
     <t>Credit Type</t>
+  </si>
+  <si>
+    <t>ZEV Class Ordering</t>
+  </si>
+  <si>
+    <t>Divisor</t>
+  </si>
+  <si>
+    <t>Final Number of Units</t>
+  </si>
+  <si>
+    <t>Initial Number of Units</t>
+  </si>
+  <si>
+    <t>Compliant</t>
   </si>
 </sst>
 </file>
@@ -464,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F98C4F-709F-BE41-A61C-7C5BE18E78C9}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -473,10 +481,12 @@
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
-    <col min="4" max="4" width="86.83203125" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,13 +494,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91F418E-62AA-B84B-ABCE-E4D97A035535}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -512,7 +537,47 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70438796-C504-964A-BE49-E27234E80981}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -521,13 +586,10 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -535,52 +597,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A603B588-451E-DE47-B4C5-80CCA31AA744}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092B32A8-1A64-2347-99F3-32905DDC8385}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="135.5" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59281AEA-3AA5-0C4E-A67E-4D6171492622}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -589,95 +634,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240610B3-BA6F-EA4D-8E64-BC14F2315C65}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092B32A8-1A64-2347-99F3-32905DDC8385}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63D4D29-49CB-FE47-AAC8-5E814C359DDB}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -694,19 +650,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -714,15 +670,132 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F2F3A0-C836-3C4C-9B76-FCF87CCE7131}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240610B3-BA6F-EA4D-8E64-BC14F2315C65}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EE9819-10C8-664D-85A7-E78A635E958F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59281AEA-3AA5-0C4E-A67E-4D6171492622}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A603B588-451E-DE47-B4C5-80CCA31AA744}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="166" customWidth="1"/>
+    <col min="1" max="1" width="135.5" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: MYR refinements (#334)
* some refinements

* second commit

* third commit
</commit_message>
<xml_diff>
--- a/next/app/model-year-report/lib/templates/assessment_template.xlsx
+++ b/next/app/model-year-report/lib/templates/assessment_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/zeva/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B1F051-C09F-0640-B40A-7D67FD51B4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1916526C-CB57-764A-9AD0-9A16661C2187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2100" windowWidth="32280" windowHeight="16940" xr2:uid="{596842B5-1F9C-BB4A-9EA7-2707F0F20405}"/>
+    <workbookView xWindow="2280" yWindow="2880" windowWidth="32280" windowHeight="16940" xr2:uid="{596842B5-1F9C-BB4A-9EA7-2707F0F20405}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="Offsets and Transfers Away" sheetId="5" r:id="rId7"/>
     <sheet name="Final Ending Balance" sheetId="3" r:id="rId8"/>
     <sheet name="Statement(s)" sheetId="4" r:id="rId9"/>
-    <sheet name="Divisor" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +35,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -45,10 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
-  <si>
-    <t>Supplier Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
   <si>
     <t>Model Year</t>
   </si>
@@ -472,50 +467,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F98C4F-709F-BE41-A61C-7C5BE18E78C9}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="24.5" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91F418E-62AA-B84B-ABCE-E4D97A035535}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -537,22 +512,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -577,19 +552,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -613,19 +588,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -650,19 +625,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -687,19 +662,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -724,19 +699,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -761,25 +736,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>